<commit_message>
Ajout références conf + script génération 51947c886c637a094c4dd6eab28ddcc7f9db7076
</commit_message>
<xml_diff>
--- a/ML/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
+++ b/ML/ig/StructureDefinition-CapaciteSavoirfaire.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-29T10:18:40+00:00</t>
+    <t>2025-10-29T11:46:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -288,17 +288,17 @@
     <t>SavoirFaire.dateAbandon</t>
   </si>
   <si>
-    <t>CapaciteSavoirfaire.exerciceProfessionnel</t>
+    <t>CapaciteSavoirfaire.ExerciceProfessionnel</t>
   </si>
   <si>
     <t xml:space="preserve">https://interop.esante.gouv.fr/ig/mos/StructureDefinition/ExerciceProfessionnel
 </t>
   </si>
   <si>
-    <t>Lien vers la classe ExerciceProfessionnel.</t>
-  </si>
-  <si>
-    <t>SavoirFaire.exerciceProfessionnel</t>
+    <t>Lien vers la classe ExerciceProfessionnel</t>
+  </si>
+  <si>
+    <t>SavoirFaire.ExerciceProfessionnel</t>
   </si>
   <si>
     <t>CapaciteSavoirfaire.capaciteSavoirFaire</t>
@@ -621,8 +621,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="33.953125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="33.953125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.98046875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.98046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>

</xml_diff>